<commit_message>
word e excel atualizados
</commit_message>
<xml_diff>
--- a/Projeto-aspetos-em-avaliacao.xlsx
+++ b/Projeto-aspetos-em-avaliacao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/teresavazao/Documents/cadeiras/IRC/Modelo-Geral-IRC-PERCIST/projeto/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CCBA4438-F1E9-4118-A9A5-0F4FBD7ACC52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCA9695D-6446-4F90-B6ED-697DEB7089F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4460" yWindow="1560" windowWidth="26840" windowHeight="15080" xr2:uid="{95692506-BAEE-D044-938B-D431CA1AA22A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="106">
   <si>
     <t>Grupo</t>
   </si>
@@ -892,7 +892,7 @@
   <dimension ref="B2:E93"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D77" sqref="D77"/>
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1630,9 +1630,12 @@
       <c r="C63" s="10" t="s">
         <v>73</v>
       </c>
+      <c r="D63" s="21" t="s">
+        <v>69</v>
+      </c>
       <c r="E63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="2:5">
@@ -1640,9 +1643,12 @@
       <c r="C64" s="10" t="s">
         <v>8</v>
       </c>
+      <c r="D64" s="21" t="s">
+        <v>70</v>
+      </c>
       <c r="E64">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="2:5" ht="15.75" customHeight="1">

</xml_diff>